<commit_message>
worked out 2D motor->torque->position,heading mafs
</commit_message>
<xml_diff>
--- a/doc/Example1D.xlsx
+++ b/doc/Example1D.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Ashwin\Code\Python\Robot Simulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Ashwin\Code\Python\Robot Simulator\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1773,11 +1773,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="216701184"/>
-        <c:axId val="216701576"/>
+        <c:axId val="407781752"/>
+        <c:axId val="407776264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="216701184"/>
+        <c:axId val="407781752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1820,7 +1820,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216701576"/>
+        <c:crossAx val="407776264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1828,7 +1828,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216701576"/>
+        <c:axId val="407776264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1879,7 +1879,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216701184"/>
+        <c:crossAx val="407781752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3559,11 +3559,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="507935856"/>
-        <c:axId val="507936640"/>
+        <c:axId val="407782928"/>
+        <c:axId val="407776656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="507935856"/>
+        <c:axId val="407782928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3606,7 +3606,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507936640"/>
+        <c:crossAx val="407776656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3614,7 +3614,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="507936640"/>
+        <c:axId val="407776656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3665,7 +3665,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507935856"/>
+        <c:crossAx val="407782928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5354,11 +5354,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="496083288"/>
-        <c:axId val="496078584"/>
+        <c:axId val="537206152"/>
+        <c:axId val="537195568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="496083288"/>
+        <c:axId val="537206152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5415,12 +5415,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496078584"/>
+        <c:crossAx val="537195568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="496078584"/>
+        <c:axId val="537195568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5477,7 +5477,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496083288"/>
+        <c:crossAx val="537206152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7176,11 +7176,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="506565736"/>
-        <c:axId val="506572008"/>
+        <c:axId val="537199096"/>
+        <c:axId val="537197920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="506565736"/>
+        <c:axId val="537199096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7237,12 +7237,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="506572008"/>
+        <c:crossAx val="537197920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="506572008"/>
+        <c:axId val="537197920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7299,7 +7299,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="506565736"/>
+        <c:crossAx val="537199096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9962,8 +9962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I262"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q273" sqref="Q273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17044,7 +17044,7 @@
         <v>1.94</v>
       </c>
       <c r="C206">
-        <f t="shared" ref="C206:C269" si="21">B206-B205</f>
+        <f t="shared" ref="C206:C262" si="21">B206-B205</f>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="D206">
@@ -17056,7 +17056,7 @@
         <v>0.11572122294036724</v>
       </c>
       <c r="F206">
-        <f t="shared" ref="F206:F269" si="24">E206/$C$7</f>
+        <f t="shared" ref="F206:F262" si="24">E206/$C$7</f>
         <v>1.7017826902995182E-2</v>
       </c>
       <c r="G206">

</xml_diff>